<commit_message>
Comments, RD2, test cases fixed -Cooper
</commit_message>
<xml_diff>
--- a/test_cases.xlsx
+++ b/test_cases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Crush\PycharmProjects\cs151-lab4-cooper_lucas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nmare\PycharmProjects\cs151-lab4-cooper_lucas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A899BD-A4E0-482F-BEE9-A38B8DD88B3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98691E2D-A341-4638-B2FF-7D138125486E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>Test Description</t>
   </si>
@@ -90,18 +90,6 @@
     <t>Cost after Coupon</t>
   </si>
   <si>
-    <t>Green Package 2 months</t>
-  </si>
-  <si>
-    <t>Blue Package 2 months</t>
-  </si>
-  <si>
-    <t>Purple Package 2 months</t>
-  </si>
-  <si>
-    <t>Green Package 3 months with additional 5 GB data</t>
-  </si>
-  <si>
     <t>green</t>
   </si>
   <si>
@@ -114,7 +102,16 @@
     <t>input: data used</t>
   </si>
   <si>
-    <t>input: months</t>
+    <t>Green Package 2 GB</t>
+  </si>
+  <si>
+    <t>Blue Package 2 GB</t>
+  </si>
+  <si>
+    <t>Purple Package</t>
+  </si>
+  <si>
+    <t>Green Package 5 GB</t>
   </si>
 </sst>
 </file>
@@ -528,22 +525,22 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" width="18.296875" customWidth="1"/>
     <col min="2" max="2" width="26.5" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="28.83203125" customWidth="1"/>
-    <col min="6" max="6" width="20.1640625" customWidth="1"/>
+    <col min="5" max="5" width="28.796875" customWidth="1"/>
+    <col min="6" max="6" width="20.19921875" customWidth="1"/>
     <col min="7" max="7" width="18.5" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="10.796875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>3</v>
       </c>
@@ -563,7 +560,7 @@
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -583,7 +580,7 @@
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
@@ -603,7 +600,7 @@
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
@@ -623,7 +620,7 @@
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -633,7 +630,7 @@
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -643,7 +640,7 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" spans="1:8" s="9" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" s="9" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
@@ -657,18 +654,16 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="31.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="C8" s="6"/>
       <c r="D8" s="6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="6" t="s">
@@ -679,16 +674,14 @@
       </c>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:8" ht="28.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="3">
-        <v>2</v>
-      </c>
+      <c r="C9" s="3"/>
       <c r="D9" s="3">
         <v>2</v>
       </c>
@@ -703,16 +696,14 @@
       </c>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:8" ht="28.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="3">
-        <v>2</v>
-      </c>
+      <c r="C10" s="3"/>
       <c r="D10" s="3">
         <v>1</v>
       </c>
@@ -727,16 +718,14 @@
       </c>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:8" ht="28.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="3">
-        <v>2</v>
-      </c>
+      <c r="C11" s="3"/>
       <c r="D11" s="3" t="s">
         <v>13</v>
       </c>
@@ -751,31 +740,29 @@
       </c>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="3">
-        <v>3</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C12" s="3"/>
       <c r="D12" s="3">
         <v>5</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="4">
-        <f>IF(D12&gt;B2,49.99+15*(D12-B5),49.99)</f>
-        <v>124.99000000000001</v>
+        <f>IF(D12&gt;B2,49.99+15*(D12-B2),49.99)</f>
+        <v>94.990000000000009</v>
       </c>
       <c r="G12" s="4">
         <f t="shared" si="0"/>
-        <v>104.99000000000001</v>
+        <v>74.990000000000009</v>
       </c>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>

</xml_diff>